<commit_message>
fixed datetime format 2
</commit_message>
<xml_diff>
--- a/Cushing_OK_WTI_Spot_Price_FOB_MonthlyFreq.xlsx
+++ b/Cushing_OK_WTI_Spot_Price_FOB_MonthlyFreq.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyITSAcademia2-Season1\PDST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MyITSAcademia2-Season1\PDST\mid-fp-pdst-s2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D904A12E-9852-4F31-883A-3170DF28561D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19ACA5FA-D974-4A6F-BA87-4DDCA8DE88E8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{09F19EC2-C3DB-41AA-A92E-47F288543683}"/>
   </bookViews>
@@ -1440,6 +1440,9 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="[$-13809]dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1451,11 +1454,13 @@
     <font>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b/>
       <sz val="10"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1485,8 +1490,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1822,7 +1829,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D22BB955-C437-45D7-BFAB-40668E9BA515}">
-  <dimension ref="A1:F466"/>
+  <dimension ref="A1:B466"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A2" sqref="A2:A466"/>
@@ -1834,7 +1841,7 @@
     <col min="2" max="2" width="48.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1842,140 +1849,125 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>31413</v>
       </c>
       <c r="B2" s="1">
         <v>22.93</v>
       </c>
-      <c r="F2" s="3"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>2</v>
       </c>
       <c r="B3" s="1">
         <v>15.46</v>
       </c>
-      <c r="F3" s="3"/>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="1">
         <v>12.61</v>
       </c>
-      <c r="F4" s="3"/>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5" s="4" t="s">
         <v>4</v>
       </c>
       <c r="B5" s="1">
         <v>12.84</v>
       </c>
-      <c r="F5" s="3"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="1">
         <v>15.38</v>
       </c>
-      <c r="F6" s="3"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
       <c r="B7" s="1">
         <v>13.43</v>
       </c>
-      <c r="F7" s="3"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8" s="4" t="s">
         <v>7</v>
       </c>
       <c r="B8" s="1">
         <v>11.59</v>
       </c>
-      <c r="F8" s="3"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B9" s="1">
         <v>15.1</v>
       </c>
-      <c r="F9" s="3"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>9</v>
       </c>
       <c r="B10" s="1">
         <v>14.87</v>
       </c>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11" s="4" t="s">
         <v>10</v>
       </c>
       <c r="B11" s="1">
         <v>14.9</v>
       </c>
-      <c r="F11" s="3"/>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
       <c r="B12" s="1">
         <v>15.22</v>
       </c>
-      <c r="F12" s="3"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
       <c r="B13" s="1">
         <v>16.11</v>
       </c>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B14" s="1">
         <v>18.649999999999999</v>
       </c>
-      <c r="F14" s="3"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
       <c r="B15" s="1">
         <v>17.75</v>
       </c>
-      <c r="F15" s="3"/>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
       <c r="B16" s="1">
         <v>18.3</v>
       </c>
-      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17" s="4" t="s">

</xml_diff>